<commit_message>
172.18.172.216 table format change
</commit_message>
<xml_diff>
--- a/172.18.152.216国家站及区域站cimiss显示.xlsx
+++ b/172.18.152.216国家站及区域站cimiss显示.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="24300" windowHeight="9540"/>
+    <workbookView windowWidth="28695" windowHeight="14850"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242">
   <si>
     <t>cimiss区域站分钟数据</t>
   </si>
@@ -391,6 +391,357 @@
   </si>
   <si>
     <t> /</t>
+  </si>
+  <si>
+    <t>区域站cimiss正点数据</t>
+  </si>
+  <si>
+    <t>区域</t>
+  </si>
+  <si>
+    <t>最高温度(℃)</t>
+  </si>
+  <si>
+    <t>最高温度时间</t>
+  </si>
+  <si>
+    <t>最低温度(℃)</t>
+  </si>
+  <si>
+    <t>最低温度时间</t>
+  </si>
+  <si>
+    <t>瞬时风速(m/s)</t>
+  </si>
+  <si>
+    <t>瞬时风向</t>
+  </si>
+  <si>
+    <t>二分风速(m/s)</t>
+  </si>
+  <si>
+    <t>二分风向</t>
+  </si>
+  <si>
+    <t>十分风速(m/s)</t>
+  </si>
+  <si>
+    <t>十分风向</t>
+  </si>
+  <si>
+    <t>最大风速(m/s)</t>
+  </si>
+  <si>
+    <t>最大风向</t>
+  </si>
+  <si>
+    <t>最大风速时间</t>
+  </si>
+  <si>
+    <t>极大风速(m/s)</t>
+  </si>
+  <si>
+    <t>极大风向</t>
+  </si>
+  <si>
+    <t>极大风速时间</t>
+  </si>
+  <si>
+    <t>湿度(%)</t>
+  </si>
+  <si>
+    <t>最低湿度(%)</t>
+  </si>
+  <si>
+    <t>最低湿度时间</t>
+  </si>
+  <si>
+    <t>气压(Pa)</t>
+  </si>
+  <si>
+    <t>最高气压(Pa)</t>
+  </si>
+  <si>
+    <t>最高气压时间</t>
+  </si>
+  <si>
+    <t>最低气压(Pa)</t>
+  </si>
+  <si>
+    <t>最低气压时间</t>
+  </si>
+  <si>
+    <t> 1</t>
+  </si>
+  <si>
+    <t> 王村</t>
+  </si>
+  <si>
+    <t> O2179</t>
+  </si>
+  <si>
+    <t> 洛阳市-洛宁县</t>
+  </si>
+  <si>
+    <t> 0</t>
+  </si>
+  <si>
+    <t> 14.7</t>
+  </si>
+  <si>
+    <t> 15.4</t>
+  </si>
+  <si>
+    <t> 11:01</t>
+  </si>
+  <si>
+    <t> 14.2</t>
+  </si>
+  <si>
+    <t> 11:26</t>
+  </si>
+  <si>
+    <t> 205</t>
+  </si>
+  <si>
+    <t> 0.1</t>
+  </si>
+  <si>
+    <t> 194</t>
+  </si>
+  <si>
+    <t> 0.6</t>
+  </si>
+  <si>
+    <t> 234</t>
+  </si>
+  <si>
+    <t> 1.4</t>
+  </si>
+  <si>
+    <t> 299</t>
+  </si>
+  <si>
+    <t> 11:39</t>
+  </si>
+  <si>
+    <t> 2.4</t>
+  </si>
+  <si>
+    <t> 329</t>
+  </si>
+  <si>
+    <t> 11:36</t>
+  </si>
+  <si>
+    <t> 2</t>
+  </si>
+  <si>
+    <t> 下峪</t>
+  </si>
+  <si>
+    <t> O2180</t>
+  </si>
+  <si>
+    <t> 12.6</t>
+  </si>
+  <si>
+    <t> 12.7</t>
+  </si>
+  <si>
+    <t> 11:48</t>
+  </si>
+  <si>
+    <t> 12.2</t>
+  </si>
+  <si>
+    <t> 11:20</t>
+  </si>
+  <si>
+    <t> 1.8</t>
+  </si>
+  <si>
+    <t> 39</t>
+  </si>
+  <si>
+    <t> 1.7</t>
+  </si>
+  <si>
+    <t> 29</t>
+  </si>
+  <si>
+    <t> 1.5</t>
+  </si>
+  <si>
+    <t> 35</t>
+  </si>
+  <si>
+    <t> 30</t>
+  </si>
+  <si>
+    <t> 2.5</t>
+  </si>
+  <si>
+    <t> 34</t>
+  </si>
+  <si>
+    <t> 11:25</t>
+  </si>
+  <si>
+    <t> 73</t>
+  </si>
+  <si>
+    <t> 72</t>
+  </si>
+  <si>
+    <t> 355</t>
+  </si>
+  <si>
+    <t> 938.2</t>
+  </si>
+  <si>
+    <t> 938.9</t>
+  </si>
+  <si>
+    <t> 301</t>
+  </si>
+  <si>
+    <t> 400</t>
+  </si>
+  <si>
+    <t>2022年6月更新</t>
+  </si>
+  <si>
+    <t>气温质控码</t>
+  </si>
+  <si>
+    <t>小时降水质控码</t>
+  </si>
+  <si>
+    <t>现在天气</t>
+  </si>
+  <si>
+    <t>缺测</t>
+  </si>
+  <si>
+    <t>缺测缺测缺测缺测缺测缺测缺测缺测</t>
+  </si>
+  <si>
+    <t>不观测和无数据</t>
+  </si>
+  <si>
+    <t> 缺测</t>
+  </si>
+  <si>
+    <t> 32.1</t>
+  </si>
+  <si>
+    <t> 32.3</t>
+  </si>
+  <si>
+    <t> 08:59</t>
+  </si>
+  <si>
+    <t> 28.8</t>
+  </si>
+  <si>
+    <t> 08:01</t>
+  </si>
+  <si>
+    <t> 3.1</t>
+  </si>
+  <si>
+    <t> 89</t>
+  </si>
+  <si>
+    <t> 3.2</t>
+  </si>
+  <si>
+    <t> 61</t>
+  </si>
+  <si>
+    <t> 3</t>
+  </si>
+  <si>
+    <t> 57</t>
+  </si>
+  <si>
+    <t> 4.2</t>
+  </si>
+  <si>
+    <t> 66</t>
+  </si>
+  <si>
+    <t> 08:10</t>
+  </si>
+  <si>
+    <t> 6.7</t>
+  </si>
+  <si>
+    <t> 08:02</t>
+  </si>
+  <si>
+    <t> 26.2</t>
+  </si>
+  <si>
+    <t> 09:00</t>
+  </si>
+  <si>
+    <t> 23.8</t>
+  </si>
+  <si>
+    <t> 5.7</t>
+  </si>
+  <si>
+    <t> 219</t>
+  </si>
+  <si>
+    <t> 5.4</t>
+  </si>
+  <si>
+    <t> 228</t>
+  </si>
+  <si>
+    <t> 5.5</t>
+  </si>
+  <si>
+    <t> 231</t>
+  </si>
+  <si>
+    <t> 7</t>
+  </si>
+  <si>
+    <t> 239</t>
+  </si>
+  <si>
+    <t> 08:13</t>
+  </si>
+  <si>
+    <t> 9.2</t>
+  </si>
+  <si>
+    <t> 245</t>
+  </si>
+  <si>
+    <t> 08:09</t>
+  </si>
+  <si>
+    <t> 56</t>
+  </si>
+  <si>
+    <t> 59</t>
+  </si>
+  <si>
+    <t> 926.5</t>
+  </si>
+  <si>
+    <t> 926.7</t>
+  </si>
+  <si>
+    <t> 42</t>
+  </si>
+  <si>
+    <t>定位</t>
   </si>
 </sst>
 </file>
@@ -403,7 +754,7 @@
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="21">
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -418,6 +769,14 @@
       <charset val="134"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
@@ -427,6 +786,37 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -448,7 +838,44 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -479,54 +906,10 @@
     </font>
     <font>
       <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -537,32 +920,8 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="35">
+  <fills count="36">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -583,13 +942,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor rgb="FFF7F7F7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -613,13 +1002,55 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -637,18 +1068,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -661,85 +1080,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -757,13 +1098,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -794,17 +1159,6 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top/>
       <bottom style="medium">
         <color theme="4"/>
@@ -823,21 +1177,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -875,6 +1214,32 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -897,10 +1262,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="19" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="17" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -909,137 +1274,137 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="16" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="32" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="26" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="26" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="29" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1063,6 +1428,33 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1408,16 +1800,21 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="B1:CM20"/>
+  <dimension ref="A1:CM43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" topLeftCell="F11" workbookViewId="0">
+      <selection activeCell="N43" sqref="N43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <cols>
     <col min="6" max="6" width="12.625" customWidth="1"/>
     <col min="7" max="7" width="11.75" customWidth="1"/>
+    <col min="11" max="11" width="16.375" customWidth="1"/>
+    <col min="12" max="12" width="18" customWidth="1"/>
+    <col min="14" max="14" width="15.875" customWidth="1"/>
+    <col min="15" max="15" width="16.625" customWidth="1"/>
+    <col min="16" max="16" width="18.125" customWidth="1"/>
     <col min="46" max="46" width="15.25" customWidth="1"/>
     <col min="47" max="47" width="14.125" customWidth="1"/>
     <col min="48" max="48" width="13.75" customWidth="1"/>
@@ -1427,7 +1824,7 @@
   </cols>
   <sheetData>
     <row r="1" customHeight="1"/>
-    <row r="2" spans="2:19">
+    <row r="2" spans="2:31">
       <c r="B2">
         <v>0</v>
       </c>
@@ -1481,6 +1878,42 @@
       </c>
       <c r="S2">
         <v>17</v>
+      </c>
+      <c r="T2">
+        <v>18</v>
+      </c>
+      <c r="U2">
+        <v>19</v>
+      </c>
+      <c r="V2">
+        <v>20</v>
+      </c>
+      <c r="W2">
+        <v>21</v>
+      </c>
+      <c r="X2">
+        <v>22</v>
+      </c>
+      <c r="Y2">
+        <v>23</v>
+      </c>
+      <c r="Z2">
+        <v>24</v>
+      </c>
+      <c r="AA2">
+        <v>25</v>
+      </c>
+      <c r="AB2">
+        <v>26</v>
+      </c>
+      <c r="AC2">
+        <v>27</v>
+      </c>
+      <c r="AD2">
+        <v>28</v>
+      </c>
+      <c r="AE2">
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="2:2">
@@ -2464,8 +2897,1613 @@
       </c>
       <c r="CM20" s="7"/>
     </row>
+    <row r="22" spans="2:11">
+      <c r="B22" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="C22" s="8"/>
+      <c r="D22" s="8"/>
+      <c r="E22" s="8"/>
+      <c r="F22" s="8"/>
+      <c r="G22" s="8"/>
+      <c r="H22" s="8"/>
+      <c r="I22" s="8"/>
+      <c r="J22" s="8"/>
+      <c r="K22" s="8"/>
+    </row>
+    <row r="23" ht="27" spans="2:31">
+      <c r="B23" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="I23" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="J23" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="K23" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="L23" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="M23" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="N23" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="O23" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="P23" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="Q23" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="R23" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="S23" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="T23" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="U23" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="V23" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="W23" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="X23" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="Y23" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="Z23" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="AA23" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="AB23" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="AC23" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="AD23" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="AE23" s="1" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="24" ht="27" spans="2:31">
+      <c r="B24" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="H24" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="I24" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="J24" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="K24" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="L24" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="M24" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="N24" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="O24" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="P24" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="Q24" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="R24" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="S24" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="T24" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="U24" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="V24" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="W24" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="X24" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="Y24" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="Z24" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="AA24" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="AB24" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="AC24" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="AD24" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="AE24" s="2" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="25" ht="27" spans="2:31">
+      <c r="B25" s="9" t="s">
+        <v>172</v>
+      </c>
+      <c r="C25" s="9" t="s">
+        <v>173</v>
+      </c>
+      <c r="D25" s="9" t="s">
+        <v>174</v>
+      </c>
+      <c r="E25" s="9" t="s">
+        <v>154</v>
+      </c>
+      <c r="F25" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="G25" s="9" t="s">
+        <v>175</v>
+      </c>
+      <c r="H25" s="9" t="s">
+        <v>176</v>
+      </c>
+      <c r="I25" s="9" t="s">
+        <v>177</v>
+      </c>
+      <c r="J25" s="9" t="s">
+        <v>178</v>
+      </c>
+      <c r="K25" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="L25" s="9" t="s">
+        <v>180</v>
+      </c>
+      <c r="M25" s="9" t="s">
+        <v>181</v>
+      </c>
+      <c r="N25" s="9" t="s">
+        <v>182</v>
+      </c>
+      <c r="O25" s="9" t="s">
+        <v>183</v>
+      </c>
+      <c r="P25" s="9" t="s">
+        <v>184</v>
+      </c>
+      <c r="Q25" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="R25" s="9" t="s">
+        <v>180</v>
+      </c>
+      <c r="S25" s="9" t="s">
+        <v>186</v>
+      </c>
+      <c r="T25" s="9" t="s">
+        <v>160</v>
+      </c>
+      <c r="U25" s="9" t="s">
+        <v>187</v>
+      </c>
+      <c r="V25" s="9" t="s">
+        <v>188</v>
+      </c>
+      <c r="W25" s="9" t="s">
+        <v>189</v>
+      </c>
+      <c r="X25" s="9" t="s">
+        <v>190</v>
+      </c>
+      <c r="Y25" s="9" t="s">
+        <v>191</v>
+      </c>
+      <c r="Z25" s="9" t="s">
+        <v>192</v>
+      </c>
+      <c r="AA25" s="9" t="s">
+        <v>193</v>
+      </c>
+      <c r="AB25" s="9" t="s">
+        <v>194</v>
+      </c>
+      <c r="AC25" s="9" t="s">
+        <v>195</v>
+      </c>
+      <c r="AD25" s="9" t="s">
+        <v>193</v>
+      </c>
+      <c r="AE25" s="9" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="27" spans="2:38">
+      <c r="B27">
+        <v>0</v>
+      </c>
+      <c r="C27">
+        <v>1</v>
+      </c>
+      <c r="D27">
+        <v>2</v>
+      </c>
+      <c r="E27">
+        <v>3</v>
+      </c>
+      <c r="F27">
+        <v>4</v>
+      </c>
+      <c r="G27">
+        <v>5</v>
+      </c>
+      <c r="H27">
+        <v>6</v>
+      </c>
+      <c r="I27">
+        <v>7</v>
+      </c>
+      <c r="J27">
+        <v>8</v>
+      </c>
+      <c r="K27">
+        <v>9</v>
+      </c>
+      <c r="L27">
+        <v>10</v>
+      </c>
+      <c r="M27">
+        <v>11</v>
+      </c>
+      <c r="N27">
+        <v>12</v>
+      </c>
+      <c r="O27">
+        <v>13</v>
+      </c>
+      <c r="P27">
+        <v>14</v>
+      </c>
+      <c r="Q27">
+        <v>15</v>
+      </c>
+      <c r="R27">
+        <v>16</v>
+      </c>
+      <c r="S27">
+        <v>17</v>
+      </c>
+      <c r="T27">
+        <v>18</v>
+      </c>
+      <c r="U27">
+        <v>19</v>
+      </c>
+      <c r="V27">
+        <v>20</v>
+      </c>
+      <c r="W27">
+        <v>21</v>
+      </c>
+      <c r="X27">
+        <v>22</v>
+      </c>
+      <c r="Y27">
+        <v>23</v>
+      </c>
+      <c r="Z27">
+        <v>24</v>
+      </c>
+      <c r="AA27">
+        <v>25</v>
+      </c>
+      <c r="AB27">
+        <v>26</v>
+      </c>
+      <c r="AC27">
+        <v>27</v>
+      </c>
+      <c r="AD27">
+        <v>28</v>
+      </c>
+      <c r="AE27">
+        <v>29</v>
+      </c>
+      <c r="AF27">
+        <v>30</v>
+      </c>
+      <c r="AG27">
+        <v>31</v>
+      </c>
+      <c r="AH27">
+        <v>32</v>
+      </c>
+      <c r="AI27">
+        <v>33</v>
+      </c>
+      <c r="AJ27">
+        <v>34</v>
+      </c>
+      <c r="AK27">
+        <v>35</v>
+      </c>
+      <c r="AL27">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="31" spans="2:3">
+      <c r="B31" s="10" t="s">
+        <v>197</v>
+      </c>
+      <c r="C31" s="11"/>
+    </row>
+    <row r="33" spans="2:2">
+      <c r="B33" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="34" spans="2:86">
+      <c r="B34" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C34" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="D34" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="E34" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="F34" s="12" t="s">
+        <v>198</v>
+      </c>
+      <c r="G34" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="H34" s="12" t="s">
+        <v>199</v>
+      </c>
+      <c r="I34" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="J34" s="12"/>
+      <c r="K34" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="L34" s="12"/>
+      <c r="M34" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="N34" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="O34" s="12"/>
+      <c r="P34" s="12"/>
+      <c r="Q34" s="12"/>
+      <c r="R34" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="S34" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="T34" s="12"/>
+      <c r="U34" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="V34" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="W34" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="X34" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="Y34" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="Z34" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="AA34" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="AB34" s="12"/>
+      <c r="AC34" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="AD34" s="12"/>
+      <c r="AE34" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="AF34" s="12"/>
+      <c r="AG34" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="AH34" s="12"/>
+      <c r="AI34" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="AJ34" s="12"/>
+      <c r="AK34" s="12"/>
+      <c r="AL34" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="AM34" s="12"/>
+      <c r="AN34" s="12"/>
+      <c r="AO34" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="AP34" s="12"/>
+      <c r="AQ34" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="AR34" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="AS34" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="AT34" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="AU34" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="AV34" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="AW34" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="AX34" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="AY34" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="AZ34" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="BA34" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="BB34" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="BC34" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="BD34" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="BE34" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="BF34" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="BG34" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="BH34" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="BI34" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="BJ34" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="BK34" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="BL34" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="BM34" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="BN34" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="BO34" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="BP34" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="BQ34" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="BR34" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="BS34" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="BT34" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="BU34" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="BV34" s="12" t="s">
+        <v>96</v>
+      </c>
+      <c r="BW34" s="12" t="s">
+        <v>200</v>
+      </c>
+      <c r="BX34" s="12" t="s">
+        <v>99</v>
+      </c>
+      <c r="BY34" s="12" t="s">
+        <v>100</v>
+      </c>
+      <c r="BZ34" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="CA34" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="CB34" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="CC34" s="12" t="s">
+        <v>104</v>
+      </c>
+      <c r="CD34" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="CE34" s="12" t="s">
+        <v>106</v>
+      </c>
+      <c r="CF34" s="12" t="s">
+        <v>107</v>
+      </c>
+      <c r="CG34" s="12" t="s">
+        <v>108</v>
+      </c>
+      <c r="CH34" s="12" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="35" spans="2:86">
+      <c r="B35" s="12"/>
+      <c r="C35" s="12"/>
+      <c r="D35" s="12"/>
+      <c r="E35" s="12"/>
+      <c r="F35" s="12"/>
+      <c r="G35" s="12"/>
+      <c r="H35" s="12"/>
+      <c r="I35" s="12" t="s">
+        <v>115</v>
+      </c>
+      <c r="J35" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="K35" s="12" t="s">
+        <v>115</v>
+      </c>
+      <c r="L35" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="M35" s="12"/>
+      <c r="N35" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="O35" s="12" t="s">
+        <v>118</v>
+      </c>
+      <c r="P35" s="12" t="s">
+        <v>119</v>
+      </c>
+      <c r="Q35" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="R35" s="12"/>
+      <c r="S35" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="T35" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="U35" s="12"/>
+      <c r="V35" s="12"/>
+      <c r="W35" s="12"/>
+      <c r="X35" s="12"/>
+      <c r="Y35" s="12"/>
+      <c r="Z35" s="12"/>
+      <c r="AA35" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="AB35" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="AC35" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="AD35" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="AE35" s="12" t="s">
+        <v>121</v>
+      </c>
+      <c r="AF35" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="AG35" s="12" t="s">
+        <v>121</v>
+      </c>
+      <c r="AH35" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="AI35" s="12" t="s">
+        <v>121</v>
+      </c>
+      <c r="AJ35" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="AK35" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="AL35" s="12" t="s">
+        <v>121</v>
+      </c>
+      <c r="AM35" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="AN35" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="AO35" s="12" t="s">
+        <v>121</v>
+      </c>
+      <c r="AP35" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="AQ35" s="12"/>
+      <c r="AR35" s="12"/>
+      <c r="AS35" s="12"/>
+      <c r="AT35" s="12"/>
+      <c r="AU35" s="12"/>
+      <c r="AV35" s="12"/>
+      <c r="AW35" s="12"/>
+      <c r="AX35" s="12"/>
+      <c r="AY35" s="12"/>
+      <c r="AZ35" s="12"/>
+      <c r="BA35" s="12"/>
+      <c r="BB35" s="12"/>
+      <c r="BC35" s="12"/>
+      <c r="BD35" s="12"/>
+      <c r="BE35" s="12"/>
+      <c r="BF35" s="12"/>
+      <c r="BG35" s="12"/>
+      <c r="BH35" s="12"/>
+      <c r="BI35" s="12"/>
+      <c r="BJ35" s="12"/>
+      <c r="BK35" s="12"/>
+      <c r="BL35" s="12"/>
+      <c r="BM35" s="12"/>
+      <c r="BN35" s="12"/>
+      <c r="BO35" s="12"/>
+      <c r="BP35" s="12"/>
+      <c r="BQ35" s="12"/>
+      <c r="BR35" s="12"/>
+      <c r="BS35" s="12"/>
+      <c r="BT35" s="12"/>
+      <c r="BU35" s="12"/>
+      <c r="BV35" s="12"/>
+      <c r="BW35" s="12"/>
+      <c r="BX35" s="12"/>
+      <c r="BY35" s="12"/>
+      <c r="BZ35" s="12"/>
+      <c r="CA35" s="12"/>
+      <c r="CB35" s="12"/>
+      <c r="CC35" s="12"/>
+      <c r="CD35" s="12"/>
+      <c r="CE35" s="12"/>
+      <c r="CF35" s="12"/>
+      <c r="CG35" s="12"/>
+      <c r="CH35" s="12"/>
+    </row>
+    <row r="36" spans="2:86">
+      <c r="B36" s="13">
+        <v>1</v>
+      </c>
+      <c r="C36" s="13">
+        <v>57065</v>
+      </c>
+      <c r="D36" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="E36" s="13">
+        <v>30.1</v>
+      </c>
+      <c r="F36" s="13">
+        <v>0</v>
+      </c>
+      <c r="G36" s="13">
+        <v>0</v>
+      </c>
+      <c r="H36" s="13">
+        <v>0</v>
+      </c>
+      <c r="I36" s="13">
+        <v>30.1</v>
+      </c>
+      <c r="J36" s="13">
+        <v>100</v>
+      </c>
+      <c r="K36" s="13">
+        <v>27.3</v>
+      </c>
+      <c r="L36" s="13">
+        <v>4</v>
+      </c>
+      <c r="M36" s="13">
+        <v>15900</v>
+      </c>
+      <c r="N36" s="13">
+        <v>16369</v>
+      </c>
+      <c r="O36" s="13">
+        <v>16244</v>
+      </c>
+      <c r="P36" s="13">
+        <v>15763</v>
+      </c>
+      <c r="Q36" s="13">
+        <v>17</v>
+      </c>
+      <c r="R36" s="13">
+        <v>51</v>
+      </c>
+      <c r="S36" s="13">
+        <v>50</v>
+      </c>
+      <c r="T36" s="13">
+        <v>56</v>
+      </c>
+      <c r="U36" s="13">
+        <v>21.8</v>
+      </c>
+      <c r="V36" s="13">
+        <v>18.9</v>
+      </c>
+      <c r="W36" s="13">
+        <v>965.5</v>
+      </c>
+      <c r="X36" s="13"/>
+      <c r="Y36" s="13"/>
+      <c r="Z36" s="13">
+        <v>1000.6</v>
+      </c>
+      <c r="AA36" s="13">
+        <v>965.8</v>
+      </c>
+      <c r="AB36" s="13">
+        <v>2</v>
+      </c>
+      <c r="AC36" s="13">
+        <v>965.5</v>
+      </c>
+      <c r="AD36" s="13">
+        <v>40</v>
+      </c>
+      <c r="AE36" s="13">
+        <v>262</v>
+      </c>
+      <c r="AF36" s="13">
+        <v>4.6</v>
+      </c>
+      <c r="AG36" s="13">
+        <v>262</v>
+      </c>
+      <c r="AH36" s="13">
+        <v>4.7</v>
+      </c>
+      <c r="AI36" s="13">
+        <v>257</v>
+      </c>
+      <c r="AJ36" s="13">
+        <v>6.8</v>
+      </c>
+      <c r="AK36" s="13">
+        <v>16</v>
+      </c>
+      <c r="AL36" s="13">
+        <v>267</v>
+      </c>
+      <c r="AM36" s="13">
+        <v>8.6</v>
+      </c>
+      <c r="AN36" s="13">
+        <v>29</v>
+      </c>
+      <c r="AO36" s="13">
+        <v>259</v>
+      </c>
+      <c r="AP36" s="13">
+        <v>6.4</v>
+      </c>
+      <c r="AQ36" s="13">
+        <v>39.2</v>
+      </c>
+      <c r="AR36" s="13">
+        <v>39.2</v>
+      </c>
+      <c r="AS36" s="13">
+        <v>100</v>
+      </c>
+      <c r="AT36" s="13">
+        <v>32.7</v>
+      </c>
+      <c r="AU36" s="13">
+        <v>1</v>
+      </c>
+      <c r="AV36" s="13">
+        <v>0</v>
+      </c>
+      <c r="AW36" s="13">
+        <v>0</v>
+      </c>
+      <c r="AX36" s="13">
+        <v>0</v>
+      </c>
+      <c r="AY36" s="13">
+        <v>0</v>
+      </c>
+      <c r="AZ36" s="13" t="s">
+        <v>201</v>
+      </c>
+      <c r="BA36" s="13" t="s">
+        <v>201</v>
+      </c>
+      <c r="BB36" s="13">
+        <v>36.8</v>
+      </c>
+      <c r="BC36" s="13">
+        <v>23.7</v>
+      </c>
+      <c r="BD36" s="13">
+        <v>3.5</v>
+      </c>
+      <c r="BE36" s="13"/>
+      <c r="BF36" s="13">
+        <v>27.2</v>
+      </c>
+      <c r="BG36" s="13">
+        <v>27.5</v>
+      </c>
+      <c r="BH36" s="13">
+        <v>28.2</v>
+      </c>
+      <c r="BI36" s="13">
+        <v>28.1</v>
+      </c>
+      <c r="BJ36" s="13">
+        <v>25.5</v>
+      </c>
+      <c r="BK36" s="13">
+        <v>20.6</v>
+      </c>
+      <c r="BL36" s="13">
+        <v>16.6</v>
+      </c>
+      <c r="BM36" s="13">
+        <v>36.1</v>
+      </c>
+      <c r="BN36" s="13">
+        <v>36.1</v>
+      </c>
+      <c r="BO36" s="13">
+        <v>100</v>
+      </c>
+      <c r="BP36" s="13">
+        <v>31.6</v>
+      </c>
+      <c r="BQ36" s="13">
+        <v>8</v>
+      </c>
+      <c r="BR36" s="13" t="s">
+        <v>201</v>
+      </c>
+      <c r="BS36" s="13" t="s">
+        <v>201</v>
+      </c>
+      <c r="BT36" s="13" t="s">
+        <v>201</v>
+      </c>
+      <c r="BU36" s="13" t="s">
+        <v>201</v>
+      </c>
+      <c r="BV36" s="13" t="s">
+        <v>202</v>
+      </c>
+      <c r="BW36" s="13">
+        <v>0</v>
+      </c>
+      <c r="BX36" s="13" t="s">
+        <v>201</v>
+      </c>
+      <c r="BY36" s="13" t="s">
+        <v>201</v>
+      </c>
+      <c r="BZ36" s="13" t="s">
+        <v>201</v>
+      </c>
+      <c r="CA36" s="13" t="s">
+        <v>203</v>
+      </c>
+      <c r="CB36" s="13" t="s">
+        <v>201</v>
+      </c>
+      <c r="CC36" s="13" t="s">
+        <v>201</v>
+      </c>
+      <c r="CD36" s="13" t="s">
+        <v>204</v>
+      </c>
+      <c r="CE36" s="13" t="s">
+        <v>204</v>
+      </c>
+      <c r="CF36" s="13" t="s">
+        <v>204</v>
+      </c>
+      <c r="CG36" s="13" t="s">
+        <v>204</v>
+      </c>
+      <c r="CH36" s="13" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="37" spans="2:2">
+      <c r="B37" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="38" ht="24" spans="2:33">
+      <c r="B38" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="C38" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="D38" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="E38" s="14" t="s">
+        <v>126</v>
+      </c>
+      <c r="F38" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="G38" s="14" t="s">
+        <v>199</v>
+      </c>
+      <c r="H38" s="14" t="s">
+        <v>115</v>
+      </c>
+      <c r="I38" s="14" t="s">
+        <v>198</v>
+      </c>
+      <c r="J38" s="14" t="s">
+        <v>127</v>
+      </c>
+      <c r="K38" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="L38" s="14" t="s">
+        <v>129</v>
+      </c>
+      <c r="M38" s="14" t="s">
+        <v>130</v>
+      </c>
+      <c r="N38" s="14" t="s">
+        <v>131</v>
+      </c>
+      <c r="O38" s="14" t="s">
+        <v>132</v>
+      </c>
+      <c r="P38" s="14" t="s">
+        <v>133</v>
+      </c>
+      <c r="Q38" s="14" t="s">
+        <v>134</v>
+      </c>
+      <c r="R38" s="14" t="s">
+        <v>135</v>
+      </c>
+      <c r="S38" s="14" t="s">
+        <v>136</v>
+      </c>
+      <c r="T38" s="14" t="s">
+        <v>137</v>
+      </c>
+      <c r="U38" s="14" t="s">
+        <v>138</v>
+      </c>
+      <c r="V38" s="14" t="s">
+        <v>139</v>
+      </c>
+      <c r="W38" s="14" t="s">
+        <v>140</v>
+      </c>
+      <c r="X38" s="14" t="s">
+        <v>141</v>
+      </c>
+      <c r="Y38" s="14" t="s">
+        <v>142</v>
+      </c>
+      <c r="Z38" s="14" t="s">
+        <v>143</v>
+      </c>
+      <c r="AA38" s="14" t="s">
+        <v>144</v>
+      </c>
+      <c r="AB38" s="14" t="s">
+        <v>145</v>
+      </c>
+      <c r="AC38" s="14" t="s">
+        <v>146</v>
+      </c>
+      <c r="AD38" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="AE38" s="14" t="s">
+        <v>148</v>
+      </c>
+      <c r="AF38" s="14" t="s">
+        <v>149</v>
+      </c>
+      <c r="AG38" s="14" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="39" ht="24" spans="2:33">
+      <c r="B39" s="15" t="s">
+        <v>151</v>
+      </c>
+      <c r="C39" s="15" t="s">
+        <v>152</v>
+      </c>
+      <c r="D39" s="15" t="s">
+        <v>153</v>
+      </c>
+      <c r="E39" s="15" t="s">
+        <v>154</v>
+      </c>
+      <c r="F39" s="15" t="s">
+        <v>155</v>
+      </c>
+      <c r="G39" s="15" t="s">
+        <v>155</v>
+      </c>
+      <c r="H39" s="15" t="s">
+        <v>205</v>
+      </c>
+      <c r="I39" s="15" t="s">
+        <v>155</v>
+      </c>
+      <c r="J39" s="15" t="s">
+        <v>206</v>
+      </c>
+      <c r="K39" s="15" t="s">
+        <v>207</v>
+      </c>
+      <c r="L39" s="15" t="s">
+        <v>208</v>
+      </c>
+      <c r="M39" s="15" t="s">
+        <v>209</v>
+      </c>
+      <c r="N39" s="15" t="s">
+        <v>210</v>
+      </c>
+      <c r="O39" s="15" t="s">
+        <v>211</v>
+      </c>
+      <c r="P39" s="15" t="s">
+        <v>212</v>
+      </c>
+      <c r="Q39" s="15" t="s">
+        <v>213</v>
+      </c>
+      <c r="R39" s="15" t="s">
+        <v>214</v>
+      </c>
+      <c r="S39" s="15" t="s">
+        <v>215</v>
+      </c>
+      <c r="T39" s="15" t="s">
+        <v>216</v>
+      </c>
+      <c r="U39" s="15" t="s">
+        <v>217</v>
+      </c>
+      <c r="V39" s="15" t="s">
+        <v>218</v>
+      </c>
+      <c r="W39" s="15" t="s">
+        <v>219</v>
+      </c>
+      <c r="X39" s="15" t="s">
+        <v>190</v>
+      </c>
+      <c r="Y39" s="15" t="s">
+        <v>220</v>
+      </c>
+      <c r="Z39" s="15" t="s">
+        <v>204</v>
+      </c>
+      <c r="AA39" s="15" t="s">
+        <v>204</v>
+      </c>
+      <c r="AB39" s="15" t="s">
+        <v>204</v>
+      </c>
+      <c r="AC39" s="15" t="s">
+        <v>204</v>
+      </c>
+      <c r="AD39" s="15" t="s">
+        <v>204</v>
+      </c>
+      <c r="AE39" s="15" t="s">
+        <v>204</v>
+      </c>
+      <c r="AF39" s="15" t="s">
+        <v>204</v>
+      </c>
+      <c r="AG39" s="15" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="40" ht="24" spans="2:33">
+      <c r="B40" s="16" t="s">
+        <v>172</v>
+      </c>
+      <c r="C40" s="16" t="s">
+        <v>173</v>
+      </c>
+      <c r="D40" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="E40" s="16" t="s">
+        <v>154</v>
+      </c>
+      <c r="F40" s="16" t="s">
+        <v>155</v>
+      </c>
+      <c r="G40" s="16" t="s">
+        <v>155</v>
+      </c>
+      <c r="H40" s="16" t="s">
+        <v>221</v>
+      </c>
+      <c r="I40" s="16" t="s">
+        <v>155</v>
+      </c>
+      <c r="J40" s="16" t="s">
+        <v>221</v>
+      </c>
+      <c r="K40" s="16" t="s">
+        <v>222</v>
+      </c>
+      <c r="L40" s="16" t="s">
+        <v>223</v>
+      </c>
+      <c r="M40" s="16" t="s">
+        <v>209</v>
+      </c>
+      <c r="N40" s="16" t="s">
+        <v>224</v>
+      </c>
+      <c r="O40" s="16" t="s">
+        <v>225</v>
+      </c>
+      <c r="P40" s="16" t="s">
+        <v>226</v>
+      </c>
+      <c r="Q40" s="16" t="s">
+        <v>227</v>
+      </c>
+      <c r="R40" s="16" t="s">
+        <v>228</v>
+      </c>
+      <c r="S40" s="16" t="s">
+        <v>229</v>
+      </c>
+      <c r="T40" s="16" t="s">
+        <v>230</v>
+      </c>
+      <c r="U40" s="16" t="s">
+        <v>231</v>
+      </c>
+      <c r="V40" s="16" t="s">
+        <v>232</v>
+      </c>
+      <c r="W40" s="16" t="s">
+        <v>233</v>
+      </c>
+      <c r="X40" s="16" t="s">
+        <v>234</v>
+      </c>
+      <c r="Y40" s="16" t="s">
+        <v>235</v>
+      </c>
+      <c r="Z40" s="16" t="s">
+        <v>236</v>
+      </c>
+      <c r="AA40" s="16" t="s">
+        <v>236</v>
+      </c>
+      <c r="AB40" s="16" t="s">
+        <v>237</v>
+      </c>
+      <c r="AC40" s="16" t="s">
+        <v>238</v>
+      </c>
+      <c r="AD40" s="16" t="s">
+        <v>239</v>
+      </c>
+      <c r="AE40" s="16" t="s">
+        <v>172</v>
+      </c>
+      <c r="AF40" s="16" t="s">
+        <v>238</v>
+      </c>
+      <c r="AG40" s="16" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="43" spans="1:91">
+      <c r="A43" t="s">
+        <v>241</v>
+      </c>
+      <c r="B43">
+        <v>0</v>
+      </c>
+      <c r="C43">
+        <v>1</v>
+      </c>
+      <c r="D43">
+        <v>2</v>
+      </c>
+      <c r="E43">
+        <v>3</v>
+      </c>
+      <c r="F43">
+        <v>4</v>
+      </c>
+      <c r="G43">
+        <v>5</v>
+      </c>
+      <c r="H43">
+        <v>6</v>
+      </c>
+      <c r="I43">
+        <v>7</v>
+      </c>
+      <c r="J43">
+        <v>8</v>
+      </c>
+      <c r="K43">
+        <v>9</v>
+      </c>
+      <c r="L43">
+        <v>10</v>
+      </c>
+      <c r="M43">
+        <v>11</v>
+      </c>
+      <c r="N43">
+        <v>12</v>
+      </c>
+      <c r="O43">
+        <v>13</v>
+      </c>
+      <c r="P43">
+        <v>14</v>
+      </c>
+      <c r="Q43">
+        <v>15</v>
+      </c>
+      <c r="R43">
+        <v>16</v>
+      </c>
+      <c r="S43">
+        <v>17</v>
+      </c>
+      <c r="T43">
+        <v>18</v>
+      </c>
+      <c r="U43">
+        <v>19</v>
+      </c>
+      <c r="V43">
+        <v>20</v>
+      </c>
+      <c r="W43">
+        <v>21</v>
+      </c>
+      <c r="X43">
+        <v>22</v>
+      </c>
+      <c r="Y43">
+        <v>23</v>
+      </c>
+      <c r="Z43">
+        <v>24</v>
+      </c>
+      <c r="AA43">
+        <v>25</v>
+      </c>
+      <c r="AB43">
+        <v>26</v>
+      </c>
+      <c r="AC43">
+        <v>27</v>
+      </c>
+      <c r="AD43">
+        <v>28</v>
+      </c>
+      <c r="AE43">
+        <v>29</v>
+      </c>
+      <c r="AF43">
+        <v>30</v>
+      </c>
+      <c r="AG43">
+        <v>31</v>
+      </c>
+      <c r="AH43">
+        <v>32</v>
+      </c>
+      <c r="AI43">
+        <v>33</v>
+      </c>
+      <c r="AJ43">
+        <v>34</v>
+      </c>
+      <c r="AK43">
+        <v>35</v>
+      </c>
+      <c r="AL43">
+        <v>36</v>
+      </c>
+      <c r="AM43">
+        <v>37</v>
+      </c>
+      <c r="AN43">
+        <v>38</v>
+      </c>
+      <c r="AO43">
+        <v>39</v>
+      </c>
+      <c r="AP43">
+        <v>40</v>
+      </c>
+      <c r="AQ43">
+        <v>41</v>
+      </c>
+      <c r="AR43">
+        <v>42</v>
+      </c>
+      <c r="AS43">
+        <v>43</v>
+      </c>
+      <c r="AT43">
+        <v>44</v>
+      </c>
+      <c r="AU43">
+        <v>45</v>
+      </c>
+      <c r="AV43">
+        <v>46</v>
+      </c>
+      <c r="AW43">
+        <v>47</v>
+      </c>
+      <c r="AX43">
+        <v>48</v>
+      </c>
+      <c r="AY43">
+        <v>49</v>
+      </c>
+      <c r="AZ43">
+        <v>50</v>
+      </c>
+      <c r="BA43">
+        <v>51</v>
+      </c>
+      <c r="BB43">
+        <v>52</v>
+      </c>
+      <c r="BC43">
+        <v>53</v>
+      </c>
+      <c r="BD43">
+        <v>54</v>
+      </c>
+      <c r="BE43">
+        <v>55</v>
+      </c>
+      <c r="BF43">
+        <v>56</v>
+      </c>
+      <c r="BG43">
+        <v>57</v>
+      </c>
+      <c r="BH43">
+        <v>58</v>
+      </c>
+      <c r="BI43">
+        <v>59</v>
+      </c>
+      <c r="BJ43">
+        <v>60</v>
+      </c>
+      <c r="BK43">
+        <v>61</v>
+      </c>
+      <c r="BL43">
+        <v>62</v>
+      </c>
+      <c r="BM43">
+        <v>63</v>
+      </c>
+      <c r="BN43">
+        <v>64</v>
+      </c>
+      <c r="BO43">
+        <v>65</v>
+      </c>
+      <c r="BP43">
+        <v>66</v>
+      </c>
+      <c r="BQ43">
+        <v>67</v>
+      </c>
+      <c r="BR43">
+        <v>68</v>
+      </c>
+      <c r="BS43">
+        <v>69</v>
+      </c>
+      <c r="BT43">
+        <v>70</v>
+      </c>
+      <c r="BU43">
+        <v>71</v>
+      </c>
+      <c r="BV43">
+        <v>72</v>
+      </c>
+      <c r="BW43">
+        <v>73</v>
+      </c>
+      <c r="BX43">
+        <v>74</v>
+      </c>
+      <c r="BY43">
+        <v>75</v>
+      </c>
+      <c r="BZ43">
+        <v>76</v>
+      </c>
+      <c r="CA43">
+        <v>77</v>
+      </c>
+      <c r="CB43">
+        <v>78</v>
+      </c>
+      <c r="CC43">
+        <v>79</v>
+      </c>
+      <c r="CD43">
+        <v>80</v>
+      </c>
+      <c r="CE43">
+        <v>81</v>
+      </c>
+      <c r="CF43">
+        <v>82</v>
+      </c>
+      <c r="CG43">
+        <v>83</v>
+      </c>
+      <c r="CH43">
+        <v>84</v>
+      </c>
+      <c r="CI43">
+        <v>85</v>
+      </c>
+      <c r="CJ43">
+        <v>86</v>
+      </c>
+      <c r="CK43">
+        <v>87</v>
+      </c>
+      <c r="CL43">
+        <v>88</v>
+      </c>
+      <c r="CM43">
+        <v>89</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="78">
+  <mergeCells count="149">
     <mergeCell ref="B4:K4"/>
     <mergeCell ref="B12:K12"/>
     <mergeCell ref="B17:K17"/>
@@ -2480,65 +4518,136 @@
     <mergeCell ref="AG18:AI18"/>
     <mergeCell ref="AJ18:AL18"/>
     <mergeCell ref="AM18:AN18"/>
+    <mergeCell ref="B22:K22"/>
+    <mergeCell ref="I34:J34"/>
+    <mergeCell ref="K34:L34"/>
+    <mergeCell ref="N34:Q34"/>
+    <mergeCell ref="S34:T34"/>
+    <mergeCell ref="AA34:AB34"/>
+    <mergeCell ref="AC34:AD34"/>
+    <mergeCell ref="AE34:AF34"/>
+    <mergeCell ref="AG34:AH34"/>
+    <mergeCell ref="AI34:AK34"/>
+    <mergeCell ref="AL34:AN34"/>
+    <mergeCell ref="AO34:AP34"/>
     <mergeCell ref="B18:B19"/>
+    <mergeCell ref="B34:B35"/>
     <mergeCell ref="C18:C19"/>
+    <mergeCell ref="C34:C35"/>
     <mergeCell ref="D18:D19"/>
+    <mergeCell ref="D34:D35"/>
     <mergeCell ref="E18:E19"/>
+    <mergeCell ref="E34:E35"/>
     <mergeCell ref="F18:F19"/>
+    <mergeCell ref="F34:F35"/>
+    <mergeCell ref="G34:G35"/>
+    <mergeCell ref="H34:H35"/>
     <mergeCell ref="K18:K19"/>
+    <mergeCell ref="M34:M35"/>
     <mergeCell ref="P18:P19"/>
+    <mergeCell ref="R34:R35"/>
     <mergeCell ref="S18:S19"/>
     <mergeCell ref="T18:T19"/>
     <mergeCell ref="U18:U19"/>
+    <mergeCell ref="U34:U35"/>
     <mergeCell ref="V18:V19"/>
+    <mergeCell ref="V34:V35"/>
     <mergeCell ref="W18:W19"/>
+    <mergeCell ref="W34:W35"/>
     <mergeCell ref="X18:X19"/>
+    <mergeCell ref="X34:X35"/>
+    <mergeCell ref="Y34:Y35"/>
+    <mergeCell ref="Z34:Z35"/>
     <mergeCell ref="AO18:AO19"/>
     <mergeCell ref="AP18:AP19"/>
     <mergeCell ref="AQ18:AQ19"/>
+    <mergeCell ref="AQ34:AQ35"/>
     <mergeCell ref="AR18:AR19"/>
+    <mergeCell ref="AR34:AR35"/>
     <mergeCell ref="AS18:AS19"/>
+    <mergeCell ref="AS34:AS35"/>
     <mergeCell ref="AT18:AT19"/>
+    <mergeCell ref="AT34:AT35"/>
     <mergeCell ref="AU18:AU19"/>
+    <mergeCell ref="AU34:AU35"/>
     <mergeCell ref="AV18:AV19"/>
+    <mergeCell ref="AV34:AV35"/>
     <mergeCell ref="AW18:AW19"/>
+    <mergeCell ref="AW34:AW35"/>
     <mergeCell ref="AX18:AX19"/>
+    <mergeCell ref="AX34:AX35"/>
     <mergeCell ref="AY18:AY19"/>
+    <mergeCell ref="AY34:AY35"/>
     <mergeCell ref="AZ18:AZ19"/>
+    <mergeCell ref="AZ34:AZ35"/>
     <mergeCell ref="BA18:BA19"/>
+    <mergeCell ref="BA34:BA35"/>
     <mergeCell ref="BB18:BB19"/>
+    <mergeCell ref="BB34:BB35"/>
     <mergeCell ref="BC18:BC19"/>
+    <mergeCell ref="BC34:BC35"/>
     <mergeCell ref="BD18:BD19"/>
+    <mergeCell ref="BD34:BD35"/>
     <mergeCell ref="BE18:BE19"/>
+    <mergeCell ref="BE34:BE35"/>
     <mergeCell ref="BF18:BF19"/>
+    <mergeCell ref="BF34:BF35"/>
     <mergeCell ref="BG18:BG19"/>
+    <mergeCell ref="BG34:BG35"/>
     <mergeCell ref="BH18:BH19"/>
+    <mergeCell ref="BH34:BH35"/>
     <mergeCell ref="BI18:BI19"/>
+    <mergeCell ref="BI34:BI35"/>
     <mergeCell ref="BJ18:BJ19"/>
+    <mergeCell ref="BJ34:BJ35"/>
     <mergeCell ref="BK18:BK19"/>
+    <mergeCell ref="BK34:BK35"/>
     <mergeCell ref="BL18:BL19"/>
+    <mergeCell ref="BL34:BL35"/>
     <mergeCell ref="BM18:BM19"/>
+    <mergeCell ref="BM34:BM35"/>
     <mergeCell ref="BN18:BN19"/>
+    <mergeCell ref="BN34:BN35"/>
     <mergeCell ref="BO18:BO19"/>
+    <mergeCell ref="BO34:BO35"/>
     <mergeCell ref="BP18:BP19"/>
+    <mergeCell ref="BP34:BP35"/>
     <mergeCell ref="BQ18:BQ19"/>
+    <mergeCell ref="BQ34:BQ35"/>
     <mergeCell ref="BR18:BR19"/>
+    <mergeCell ref="BR34:BR35"/>
     <mergeCell ref="BS18:BS19"/>
+    <mergeCell ref="BS34:BS35"/>
     <mergeCell ref="BT18:BT19"/>
+    <mergeCell ref="BT34:BT35"/>
     <mergeCell ref="BU18:BU19"/>
+    <mergeCell ref="BU34:BU35"/>
     <mergeCell ref="BV18:BV19"/>
+    <mergeCell ref="BV34:BV35"/>
     <mergeCell ref="BW18:BW19"/>
+    <mergeCell ref="BW34:BW35"/>
     <mergeCell ref="BX18:BX19"/>
+    <mergeCell ref="BX34:BX35"/>
     <mergeCell ref="BY18:BY19"/>
+    <mergeCell ref="BY34:BY35"/>
     <mergeCell ref="BZ18:BZ19"/>
+    <mergeCell ref="BZ34:BZ35"/>
     <mergeCell ref="CA18:CA19"/>
+    <mergeCell ref="CA34:CA35"/>
     <mergeCell ref="CB18:CB19"/>
+    <mergeCell ref="CB34:CB35"/>
     <mergeCell ref="CC18:CC19"/>
+    <mergeCell ref="CC34:CC35"/>
     <mergeCell ref="CD18:CD19"/>
+    <mergeCell ref="CD34:CD35"/>
     <mergeCell ref="CE18:CE19"/>
+    <mergeCell ref="CE34:CE35"/>
     <mergeCell ref="CF18:CF19"/>
+    <mergeCell ref="CF34:CF35"/>
     <mergeCell ref="CG18:CG19"/>
+    <mergeCell ref="CG34:CG35"/>
     <mergeCell ref="CH18:CH19"/>
+    <mergeCell ref="CH34:CH35"/>
     <mergeCell ref="CI18:CI19"/>
     <mergeCell ref="CJ18:CJ19"/>
     <mergeCell ref="CK18:CK19"/>

</xml_diff>